<commit_message>
Nuevas Vistas de transformacion y vistas de modelo
</commit_message>
<xml_diff>
--- a/04_doc/DiccionarioTablas.xlsx
+++ b/04_doc/DiccionarioTablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago Nieri\Desktop\ProyectoAdventureWorks\04_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E05AC283-653C-45FD-81EB-23C4A6F43158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1C55EF-CF0D-475F-A2C1-2A7A3136665E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DFCBA9B-049D-443C-93D5-EC2788858A55}"/>
   </bookViews>
@@ -1297,7 +1297,7 @@
   <dimension ref="A1:H345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E360" sqref="E360"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>